<commit_message>
Update: Commit changes to expense-analysis.xlsx for data consistency
</commit_message>
<xml_diff>
--- a/public/expense-analysis.xlsx
+++ b/public/expense-analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kotzbauer/-expense_management_analytics-RMT/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCBC6ACE-AEEA-F149-8DB3-BF2325583D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{556C5853-36B3-5146-AF79-BBAA974293AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3740" yWindow="760" windowWidth="24160" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2920" yWindow="760" windowWidth="25800" windowHeight="16900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -214,6 +214,12 @@
     <t xml:space="preserve">      612100 Medical Billing</t>
   </si>
   <si>
+    <t xml:space="preserve">      617350 Business loan interest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Total 617300 Interest Expense</t>
+  </si>
+  <si>
     <t xml:space="preserve">      612400 Consulting Fees</t>
   </si>
   <si>
@@ -221,12 +227,6 @@
   </si>
   <si>
     <t xml:space="preserve">   618100 Cleaning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      617350 Business loan interest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Total 617300 Interest Expense</t>
   </si>
   <si>
     <t xml:space="preserve">   430000 Medical Services (PC)</t>
@@ -767,11 +767,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+    <sheetView tabSelected="1" topLeftCell="T4" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="29" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -3815,10 +3846,10 @@
         <v>0</v>
       </c>
       <c r="F36">
-        <v>4164.45</v>
+        <v>1108</v>
       </c>
       <c r="G36">
-        <v>4000</v>
+        <v>9972</v>
       </c>
       <c r="H36">
         <v>2</v>
@@ -3830,7 +3861,7 @@
         <v>0</v>
       </c>
       <c r="K36">
-        <v>1360.741666666667</v>
+        <v>1846.666666666667</v>
       </c>
       <c r="L36">
         <v>0</v>
@@ -3845,28 +3876,28 @@
         <v>109</v>
       </c>
       <c r="P36">
-        <v>1360.741666666667</v>
+        <v>1846.666666666667</v>
       </c>
       <c r="Q36">
-        <v>385.24635969864238</v>
+        <v>522.81900991015414</v>
       </c>
       <c r="R36">
-        <v>1360.741666666667</v>
+        <v>1846.666666666667</v>
       </c>
       <c r="S36">
-        <v>832.89</v>
+        <v>221.6</v>
       </c>
       <c r="T36">
-        <v>1360.741666666667</v>
+        <v>1846.666666666667</v>
       </c>
       <c r="U36">
-        <v>3167.11</v>
+        <v>9750.4</v>
       </c>
       <c r="V36">
-        <v>3.8025549592383152</v>
+        <v>44</v>
       </c>
       <c r="W36">
-        <v>2.0202886703283549</v>
+        <v>23.377098410762638</v>
       </c>
       <c r="X36" t="s">
         <v>115</v>
@@ -3875,7 +3906,7 @@
         <v>119</v>
       </c>
       <c r="AA36" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="AB36" t="s">
         <v>125</v>
@@ -3889,25 +3920,25 @@
         <v>65</v>
       </c>
       <c r="B37">
-        <v>2937.12</v>
+        <v>0</v>
       </c>
       <c r="C37">
-        <v>569.99</v>
+        <v>0</v>
       </c>
       <c r="D37">
-        <v>1567.98</v>
+        <v>0</v>
       </c>
       <c r="E37">
-        <v>385.98</v>
+        <v>0</v>
       </c>
       <c r="F37">
-        <v>210</v>
+        <v>1372.56</v>
       </c>
       <c r="G37">
-        <v>2185.8200000000002</v>
+        <v>9972</v>
       </c>
       <c r="H37">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I37" t="b">
         <v>0</v>
@@ -3916,52 +3947,52 @@
         <v>0</v>
       </c>
       <c r="K37">
-        <v>1309.481666666667</v>
+        <v>1890.76</v>
       </c>
       <c r="L37">
-        <v>7.8200000000000006E-2</v>
+        <v>0</v>
       </c>
       <c r="M37">
-        <v>-0.2848</v>
+        <v>0</v>
       </c>
       <c r="N37">
-        <v>720.70956743936449</v>
+        <v>0</v>
       </c>
       <c r="O37" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="P37">
-        <v>1309.481666666667</v>
+        <v>1890.76</v>
       </c>
       <c r="Q37">
-        <v>370.7338854488259</v>
+        <v>535.30249341753961</v>
       </c>
       <c r="R37">
-        <v>1309.481666666667</v>
+        <v>1890.76</v>
       </c>
       <c r="S37">
-        <v>1134.2139999999999</v>
+        <v>274.512</v>
       </c>
       <c r="T37">
-        <v>1309.481666666667</v>
+        <v>1890.76</v>
       </c>
       <c r="U37">
-        <v>1051.606</v>
+        <v>9697.4879999999994</v>
       </c>
       <c r="V37">
-        <v>0.92716718361790651</v>
+        <v>35.326280818324882</v>
       </c>
       <c r="W37">
-        <v>0.49260178396966903</v>
+        <v>18.768771435823119</v>
       </c>
       <c r="X37" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="Z37" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AA37" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="AB37" t="s">
         <v>125</v>
@@ -3975,25 +4006,25 @@
         <v>66</v>
       </c>
       <c r="B38">
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="C38">
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="D38">
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="E38">
         <v>0</v>
       </c>
       <c r="F38">
-        <v>1050</v>
+        <v>4164.45</v>
       </c>
       <c r="G38">
-        <v>900</v>
+        <v>4000</v>
       </c>
       <c r="H38">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I38" t="b">
         <v>0</v>
@@ -4002,52 +4033,52 @@
         <v>0</v>
       </c>
       <c r="K38">
-        <v>675</v>
+        <v>1360.741666666667</v>
       </c>
       <c r="L38">
-        <v>0.52849999999999997</v>
+        <v>0</v>
       </c>
       <c r="M38">
-        <v>0.12690000000000001</v>
+        <v>0</v>
       </c>
       <c r="N38">
-        <v>356.98255338258872</v>
+        <v>0</v>
       </c>
       <c r="O38" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="P38">
-        <v>675</v>
+        <v>1360.741666666667</v>
       </c>
       <c r="Q38">
-        <v>191.1026164382784</v>
+        <v>385.24635969864238</v>
       </c>
       <c r="R38">
-        <v>675</v>
+        <v>1360.741666666667</v>
       </c>
       <c r="S38">
-        <v>630</v>
+        <v>832.89</v>
       </c>
       <c r="T38">
-        <v>675</v>
+        <v>1360.741666666667</v>
       </c>
       <c r="U38">
-        <v>270</v>
+        <v>3167.11</v>
       </c>
       <c r="V38">
-        <v>0.42857142857142849</v>
+        <v>3.8025549592383152</v>
       </c>
       <c r="W38">
-        <v>0.2276990104944413</v>
+        <v>2.0202886703283549</v>
       </c>
       <c r="X38" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="Z38" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AA38" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AB38" t="s">
         <v>125</v>
@@ -4061,25 +4092,25 @@
         <v>67</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>2937.12</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>569.99</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>1567.98</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>385.98</v>
       </c>
       <c r="F39">
-        <v>1108</v>
+        <v>210</v>
       </c>
       <c r="G39">
-        <v>9972</v>
+        <v>2185.8200000000002</v>
       </c>
       <c r="H39">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I39" t="b">
         <v>0</v>
@@ -4088,55 +4119,55 @@
         <v>0</v>
       </c>
       <c r="K39">
-        <v>1846.666666666667</v>
+        <v>1309.481666666667</v>
       </c>
       <c r="L39">
-        <v>0</v>
+        <v>7.8200000000000006E-2</v>
       </c>
       <c r="M39">
-        <v>0</v>
+        <v>-0.2848</v>
       </c>
       <c r="N39">
-        <v>0</v>
+        <v>720.70956743936449</v>
       </c>
       <c r="O39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P39">
-        <v>1846.666666666667</v>
+        <v>1309.481666666667</v>
       </c>
       <c r="Q39">
-        <v>522.81900991015414</v>
+        <v>370.7338854488259</v>
       </c>
       <c r="R39">
-        <v>1846.666666666667</v>
+        <v>1309.481666666667</v>
       </c>
       <c r="S39">
-        <v>221.6</v>
+        <v>1134.2139999999999</v>
       </c>
       <c r="T39">
-        <v>1846.666666666667</v>
+        <v>1309.481666666667</v>
       </c>
       <c r="U39">
-        <v>9750.4</v>
+        <v>1051.606</v>
       </c>
       <c r="V39">
-        <v>44</v>
+        <v>0.92716718361790651</v>
       </c>
       <c r="W39">
-        <v>23.377098410762638</v>
+        <v>0.49260178396966903</v>
       </c>
       <c r="X39" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="Z39" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="AA39" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="AB39" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="AD39">
         <v>38</v>
@@ -4147,25 +4178,25 @@
         <v>68</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40">
-        <v>1372.56</v>
+        <v>1050</v>
       </c>
       <c r="G40">
-        <v>9972</v>
+        <v>900</v>
       </c>
       <c r="H40">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I40" t="b">
         <v>0</v>
@@ -4174,55 +4205,55 @@
         <v>0</v>
       </c>
       <c r="K40">
-        <v>1890.76</v>
+        <v>675</v>
       </c>
       <c r="L40">
-        <v>0</v>
+        <v>0.52849999999999997</v>
       </c>
       <c r="M40">
-        <v>0</v>
+        <v>0.12690000000000001</v>
       </c>
       <c r="N40">
-        <v>0</v>
+        <v>356.98255338258872</v>
       </c>
       <c r="O40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P40">
-        <v>1890.76</v>
+        <v>675</v>
       </c>
       <c r="Q40">
-        <v>535.30249341753961</v>
+        <v>191.1026164382784</v>
       </c>
       <c r="R40">
-        <v>1890.76</v>
+        <v>675</v>
       </c>
       <c r="S40">
-        <v>274.512</v>
+        <v>630</v>
       </c>
       <c r="T40">
-        <v>1890.76</v>
+        <v>675</v>
       </c>
       <c r="U40">
-        <v>9697.4879999999994</v>
+        <v>270</v>
       </c>
       <c r="V40">
-        <v>35.326280818324882</v>
+        <v>0.42857142857142849</v>
       </c>
       <c r="W40">
-        <v>18.768771435823119</v>
+        <v>0.2276990104944413</v>
       </c>
       <c r="X40" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="Z40" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="AA40" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="AB40" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="AD40">
         <v>39</v>

</xml_diff>